<commit_message>
Bob ia funcionando e adicinando arquivos da web data viz
</commit_message>
<xml_diff>
--- a/Tecnologia da Informação/Product Backlog & Gráfico de Burndown - BeeTech.xlsx
+++ b/Tecnologia da Informação/Product Backlog & Gráfico de Burndown - BeeTech.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\beetech\Sprint_2\Tecnologia da Informação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\Sprint_3\Tecnologia da Informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB588CCD-5F0B-4B9D-9529-2FDE958E84DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B48AC3-DC24-48D0-BAF1-4DFB8EA9B37A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F13FE21-3909-4024-9E51-F6B5B91CD81C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="141">
   <si>
     <t>PRODUCT BACKLOG - BEETECH</t>
   </si>
@@ -369,63 +369,9 @@
     <t>Reformulação visual do protótipo do site</t>
   </si>
   <si>
-    <t>Documentação final do projeto</t>
-  </si>
-  <si>
-    <t>Melhorar e finalizar toda e qualquer pendencia relacionada a documentação</t>
-  </si>
-  <si>
     <t>SPRINT3</t>
   </si>
   <si>
-    <t>Prévia da solução+apresentação</t>
-  </si>
-  <si>
-    <t>Preparar apresentação final do projeto com todas as conexões exigidas</t>
-  </si>
-  <si>
-    <t>Site institucional: Na nuvem conectado no BD</t>
-  </si>
-  <si>
-    <t>Configurar a conexão do Site com o banco de dados</t>
-  </si>
-  <si>
-    <t>Dashboard: Na nuvem conectado no BD</t>
-  </si>
-  <si>
-    <t>Configurar a conexão da Dashboard com a API/Banco de dados</t>
-  </si>
-  <si>
-    <t>Tela de Cadastro/Login: Na nuvem conectado no BD</t>
-  </si>
-  <si>
-    <t>Configurar a tela de Cadastro/Login com os dados inseridos no banco de dados</t>
-  </si>
-  <si>
-    <t>Modelagem Lógica do Projeto: Final</t>
-  </si>
-  <si>
-    <t>Criar versão final do diagrama de banco de dados</t>
-  </si>
-  <si>
-    <t>Tabelas em um Banco de Dados (Final)</t>
-  </si>
-  <si>
-    <t>Modificar ou atualizar a versão final do script do banco de dados do projeto</t>
-  </si>
-  <si>
-    <t>API conectada a Dashboard</t>
-  </si>
-  <si>
-    <t>Configurar e conectar API do sensor com a Dashboard</t>
-  </si>
-  <si>
-    <t>Rodar Projeto na Virtual Machine</t>
-  </si>
-  <si>
-    <t>Configurar e fazer funcionar o projeto dentro de um ambiente virtual da VM</t>
-  </si>
-  <si>
     <t>Atualizar conforme banco de dados novo</t>
   </si>
   <si>
@@ -436,6 +382,87 @@
   </si>
   <si>
     <t>Sprint4</t>
+  </si>
+  <si>
+    <t>Manual de Instalação</t>
+  </si>
+  <si>
+    <t>Doc. Final do Projeto</t>
+  </si>
+  <si>
+    <t>PPT apresentação do projeto</t>
+  </si>
+  <si>
+    <t>Site intitucional - Versão final</t>
+  </si>
+  <si>
+    <t>Cadastro,Login e dashboard, conectado com BD</t>
+  </si>
+  <si>
+    <t>Fluxgrama do processo de atendimento</t>
+  </si>
+  <si>
+    <t>Ferramenta do processo de atendimento</t>
+  </si>
+  <si>
+    <t>Documento de gestão de mudanças</t>
+  </si>
+  <si>
+    <t>Modelagem Lógica (final)</t>
+  </si>
+  <si>
+    <t>Criação das tabelas</t>
+  </si>
+  <si>
+    <t>Views para a dashboard</t>
+  </si>
+  <si>
+    <t>Solução de Iot</t>
+  </si>
+  <si>
+    <t>Distribuir solução</t>
+  </si>
+  <si>
+    <t>Criar o documento direcionado a equipe de instalação da nossa solução</t>
+  </si>
+  <si>
+    <t>Aprimorar a documentação do Projeto para a etapa final</t>
+  </si>
+  <si>
+    <t>Criar o powerpoint de apresentação do projeto</t>
+  </si>
+  <si>
+    <t>Terminar de realizar as implementações e melhorias para o site institucional</t>
+  </si>
+  <si>
+    <t>Conectar o cadastro, login e a dashboard ao banco de dados</t>
+  </si>
+  <si>
+    <t>Criar o fluxograma dos processos de atendimento ao cliente</t>
+  </si>
+  <si>
+    <t>Personalizar o Jira com a identidade visual da beetech e o adicionar os procesos de atendimento</t>
+  </si>
+  <si>
+    <t>Criar o documento GMUD</t>
+  </si>
+  <si>
+    <t>Criar a modelagem lógica do banco de dados DER</t>
+  </si>
+  <si>
+    <t>Desenvolver o código do banco de dados seguindo a modelagem lógica</t>
+  </si>
+  <si>
+    <t>Desenvolver as Views do banco de dados que serão utilizadas pela API</t>
+  </si>
+  <si>
+    <t>Conectar o banco de dados com o arduino</t>
+  </si>
+  <si>
+    <t>Distribuir a solução em duas maquinas, separando o banco de dados e aplicação e a outra para a coleta dos dados</t>
+  </si>
+  <si>
+    <t>GG</t>
   </si>
 </sst>
 </file>
@@ -654,15 +681,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -674,6 +692,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1983,8 +2010,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BF696E1-E460-4395-A8F6-CAA0467D7A56}" name="Tabela1" displayName="Tabela1" ref="A2:H52" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
-  <autoFilter ref="A2:H52" xr:uid="{2BF696E1-E460-4395-A8F6-CAA0467D7A56}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2BF696E1-E460-4395-A8F6-CAA0467D7A56}" name="Tabela1" displayName="Tabela1" ref="A2:H56" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
+  <autoFilter ref="A2:H56" xr:uid="{2BF696E1-E460-4395-A8F6-CAA0467D7A56}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{6ECC6F81-630B-49D3-805B-E9FE3D799D3D}" name="REQUISITO" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1D058733-D303-4135-A124-29464DC33A73}" name="DESCRIÇÃO" dataDxfId="6"/>
@@ -2323,8 +2350,8 @@
   </sheetPr>
   <dimension ref="A1:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" zoomScale="65" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="66" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2350,16 +2377,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1">
       <c r="A2" s="6" t="s">
@@ -2872,13 +2899,13 @@
       <c r="H20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="15"/>
-      <c r="M20" s="15"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
     </row>
     <row r="21" spans="1:16" ht="30" customHeight="1">
       <c r="A21" s="3" t="s">
@@ -2913,7 +2940,7 @@
         <v>59</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="N21" s="13" t="s">
         <v>60</v>
@@ -2921,7 +2948,7 @@
       <c r="O21" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="P21" s="19"/>
+      <c r="P21" s="16"/>
     </row>
     <row r="22" spans="1:16" ht="30" customHeight="1">
       <c r="A22" s="3" t="s">
@@ -2952,21 +2979,21 @@
       <c r="K22" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="L22" s="18">
+      <c r="L22" s="15">
         <f>SUM(L23:L26)</f>
-        <v>430</v>
-      </c>
-      <c r="M22" s="18">
+        <v>459</v>
+      </c>
+      <c r="M22" s="15">
         <f>SUM(M23:M26)</f>
         <v>430</v>
       </c>
-      <c r="N22" s="18">
+      <c r="N22" s="15">
         <f>SUM(N23:N26)</f>
         <v>430</v>
       </c>
       <c r="O22" s="13">
         <f>SUM(L22-N22)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="30" customHeight="1">
@@ -3091,7 +3118,7 @@
       </c>
       <c r="L25" s="13">
         <f>SUMIF(Tabela1[SPRINT],"SPRINT3",Tabela1[TAM('#)])</f>
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="M25" s="13">
         <v>117</v>
@@ -3101,7 +3128,7 @@
       </c>
       <c r="O25" s="13">
         <f>SUM(L25-N25)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="30" customHeight="1">
@@ -3130,17 +3157,17 @@
       <c r="H26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="20" t="s">
-        <v>131</v>
-      </c>
-      <c r="L26" s="21">
+      <c r="K26" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="L26" s="18">
         <v>0</v>
       </c>
-      <c r="M26" s="20">
+      <c r="M26" s="17">
         <v>0</v>
       </c>
-      <c r="N26" s="21"/>
-      <c r="O26" s="20">
+      <c r="N26" s="18"/>
+      <c r="O26" s="17">
         <v>0</v>
       </c>
     </row>
@@ -3578,10 +3605,10 @@
     </row>
     <row r="43" spans="1:8" ht="30" customHeight="1">
       <c r="A43" s="3" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>17</v>
@@ -3605,10 +3632,10 @@
     </row>
     <row r="44" spans="1:8" ht="30" customHeight="1">
       <c r="A44" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>17</v>
@@ -3624,7 +3651,7 @@
         <v>1</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H44" s="14" t="s">
         <v>57</v>
@@ -3632,26 +3659,26 @@
     </row>
     <row r="45" spans="1:8" ht="30" customHeight="1">
       <c r="A45" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E45" s="5">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F45" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H45" s="8" t="s">
         <v>57</v>
@@ -3659,26 +3686,26 @@
     </row>
     <row r="46" spans="1:8" ht="30" customHeight="1">
       <c r="A46" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="E46" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F46" s="2">
         <v>1</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H46" s="8" t="s">
         <v>57</v>
@@ -3686,13 +3713,13 @@
     </row>
     <row r="47" spans="1:8" ht="30" customHeight="1">
       <c r="A47" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D47" s="2" t="s">
         <v>31</v>
@@ -3705,7 +3732,7 @@
         <v>1</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H47" s="8" t="s">
         <v>57</v>
@@ -3716,10 +3743,10 @@
         <v>118</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>31</v>
@@ -3732,7 +3759,7 @@
         <v>1</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H48" s="8" t="s">
         <v>57</v>
@@ -3740,10 +3767,10 @@
     </row>
     <row r="49" spans="1:8" ht="30" customHeight="1">
       <c r="A49" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>17</v>
@@ -3759,18 +3786,18 @@
         <v>2</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H49" s="8" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="30" customHeight="1">
       <c r="A50" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>17</v>
@@ -3786,7 +3813,7 @@
         <v>2</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H50" s="8" t="s">
         <v>57</v>
@@ -3794,26 +3821,26 @@
     </row>
     <row r="51" spans="1:8" ht="30" customHeight="1">
       <c r="A51" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E51" s="5">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F51" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H51" s="8" t="s">
         <v>57</v>
@@ -3821,13 +3848,13 @@
     </row>
     <row r="52" spans="1:8" ht="30" customHeight="1">
       <c r="A52" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>12</v>
@@ -3840,56 +3867,119 @@
         <v>1</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H52" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-    </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+    <row r="53" spans="1:8" ht="25.05" customHeight="1">
+      <c r="A53" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" s="5">
+        <f>IF(D53="P",5,IF(D53="PP",3,IF(D53="M",8,IF(D53="G",13,IF(D53="GG",21,"")))))</f>
+        <v>8</v>
+      </c>
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="25.05" customHeight="1">
+      <c r="A54" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54" s="5">
+        <f>IF(D54="P",5,IF(D54="PP",3,IF(D54="M",8,IF(D54="G",13,IF(D54="GG",21,"")))))</f>
+        <v>8</v>
+      </c>
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="25.05" customHeight="1">
+      <c r="A55" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E55" s="5">
+        <f>IF(D55="P",5,IF(D55="PP",3,IF(D55="M",8,IF(D55="G",13,IF(D55="GG",21,"")))))</f>
+        <v>21</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="25.05" customHeight="1">
+      <c r="A56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="5">
+        <f>IF(D56="P",5,IF(D56="PP",3,IF(D56="M",8,IF(D56="G",13,IF(D56="GG",21,"")))))</f>
+        <v>13</v>
+      </c>
+      <c r="F56" s="2">
+        <v>2</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H56" s="10" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="62" spans="1:8">
       <c r="A62" s="1"/>
@@ -3932,7 +4022,7 @@
     <mergeCell ref="K20:O20"/>
     <mergeCell ref="A1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H52">
+  <conditionalFormatting sqref="H3:H56">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
       <formula>"FINALIZADO"</formula>
     </cfRule>
@@ -4112,20 +4202,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8497f9ae-9c71-438c-b553-1e6fe8b1acb0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4147,6 +4237,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E306DC-4D82-4FE5-B96D-A09D99E18E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0432D9B1-72E5-4E34-937B-239DA2CDF102}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4160,12 +4258,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{33E306DC-4D82-4FE5-B96D-A09D99E18E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>